<commit_message>
ganti layout master barang harga bertingkat
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangBertingkat.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangBertingkat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8151D501-F1C9-47E8-AE7D-C72D895D9F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C20CE46-6ECD-4F5E-B79A-C6FC6C91EB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,6 @@
     <t>NAMABARANG</t>
   </si>
   <si>
-    <t>JENISBARANG</t>
-  </si>
-  <si>
-    <t>MERKBARANG</t>
-  </si>
-  <si>
     <t>SATUAN</t>
   </si>
   <si>
@@ -80,6 +74,12 @@
   </si>
   <si>
     <t>RAK 1</t>
+  </si>
+  <si>
+    <t>KATEGORI</t>
+  </si>
+  <si>
+    <t>SUBKATEGORI</t>
   </si>
 </sst>
 </file>
@@ -484,24 +484,25 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="34.140625" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -509,57 +510,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -586,10 +587,10 @@
         <v>7916248854</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>